<commit_message>
chore: add the api key in code
</commit_message>
<xml_diff>
--- a/dist/countries_info.xlsx
+++ b/dist/countries_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoine.thirion\Documents\Developpement\PoC EDF\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644D4D0C-4183-4584-8685-83E68634E7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74320234-1C92-456D-9703-77883971FCE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>